<commit_message>
updated change details for CR11
</commit_message>
<xml_diff>
--- a/etc/ap242/AP242ed2_CR11_WG_Numbers.xlsx
+++ b/etc/ap242/AP242ed2_CR11_WG_Numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="-18400" windowWidth="13660" windowHeight="15680" tabRatio="500"/>
+    <workbookView xWindow="-9700" yWindow="-18340" windowWidth="12280" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="klt" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="424">
   <si>
     <t>N8573</t>
   </si>
@@ -1248,13 +1248,91 @@
   </si>
   <si>
     <t>Fabrication_joint</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>explicit_constraints</t>
+  </si>
+  <si>
+    <t>extruded_structure_cross_section</t>
+  </si>
+  <si>
+    <t>machining_features</t>
+  </si>
+  <si>
+    <t>physical_unit_2d_shape</t>
+  </si>
+  <si>
+    <t>Product_as_individual_assembly_and_test</t>
+  </si>
+  <si>
+    <t>Primitive_solids</t>
+  </si>
+  <si>
+    <t>Point_direction_model</t>
+  </si>
+  <si>
+    <t>Planned_characteristic</t>
+  </si>
+  <si>
+    <t>Parametric_representation</t>
+  </si>
+  <si>
+    <t>Parameterization_and_variational_representation</t>
+  </si>
+  <si>
+    <t>Numeric_function</t>
+  </si>
+  <si>
+    <t>Numeric_expression</t>
+  </si>
+  <si>
+    <t>Measure_representation</t>
+  </si>
+  <si>
+    <t>Manufacturing_configuration_effectivity</t>
+  </si>
+  <si>
+    <t>Manifold_surface</t>
+  </si>
+  <si>
+    <t>Manifold_subsurface</t>
+  </si>
+  <si>
+    <t>Layered_interconnect_complex_template</t>
+  </si>
+  <si>
+    <t>Interconnect_module_to_assembly_module_relationship</t>
+  </si>
+  <si>
+    <t>Inertia_characteristics</t>
+  </si>
+  <si>
+    <t>Geometrically_bounded_surface</t>
+  </si>
+  <si>
+    <t>Geometric_constraints</t>
+  </si>
+  <si>
+    <t>N8821</t>
+  </si>
+  <si>
+    <t>N8822</t>
+  </si>
+  <si>
+    <t>solid_with_local_modification</t>
+  </si>
+  <si>
+    <t>tessellated_geometry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1312,8 +1390,13 @@
       <name val="Cambria"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1326,8 +1409,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1350,8 +1439,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="553">
+  <cellStyleXfs count="591">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1905,8 +2007,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1929,8 +2069,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="553">
+  <cellStyles count="591">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2207,6 +2352,25 @@
     <cellStyle name="Lien hypertexte" xfId="547" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="549" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="589" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2483,6 +2647,25 @@
     <cellStyle name="Lien hypertexte visité" xfId="548" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="550" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="590" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2814,17 +2997,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="E106" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="9.83203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="15" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="9.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" collapsed="1"/>
     <col min="6" max="6" width="6" style="3" customWidth="1"/>
     <col min="7" max="7" width="3.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="7.5" style="3" bestFit="1" customWidth="1"/>
@@ -6453,19 +6636,19 @@
         <v>97</v>
       </c>
       <c r="F117" s="6">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H117" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I117" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K117" s="8">
         <v>42248</v>
@@ -6495,7 +6678,7 @@
         <v>336</v>
       </c>
       <c r="J118" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K118" s="8">
         <v>42248</v>
@@ -6525,7 +6708,7 @@
         <v>336</v>
       </c>
       <c r="J119" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K119" s="8">
         <v>42248</v>
@@ -6543,19 +6726,19 @@
         <v>97</v>
       </c>
       <c r="F120" s="6">
-        <v>1527</v>
+        <v>1004</v>
       </c>
       <c r="G120" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H120" s="6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I120" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J120" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K120" s="8">
         <v>42248</v>
@@ -6572,13 +6755,21 @@
       <c r="E121" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F121" s="6"/>
+      <c r="F121" s="6">
+        <v>1527</v>
+      </c>
       <c r="G121" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H121" s="6"/>
-      <c r="I121" s="6"/>
-      <c r="J121" s="4"/>
+      <c r="H121" s="6">
+        <v>2</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="J121" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K121" s="8">
         <v>42248</v>
       </c>
@@ -6594,13 +6785,21 @@
       <c r="E122" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F122" s="6"/>
+      <c r="F122" s="6">
+        <v>1064</v>
+      </c>
       <c r="G122" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
-      <c r="J122" s="4"/>
+      <c r="H122" s="6">
+        <v>2</v>
+      </c>
+      <c r="I122" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="J122" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K122" s="8">
         <v>42248</v>
       </c>
@@ -6616,13 +6815,21 @@
       <c r="E123" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F123" s="6"/>
+      <c r="F123" s="6">
+        <v>1788</v>
+      </c>
       <c r="G123" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H123" s="6"/>
-      <c r="I123" s="6"/>
-      <c r="J123" s="4"/>
+      <c r="H123" s="6">
+        <v>2</v>
+      </c>
+      <c r="I123" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="J123" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K123" s="8">
         <v>42248</v>
       </c>
@@ -6638,13 +6845,21 @@
       <c r="E124" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F124" s="6"/>
+      <c r="F124" s="6">
+        <v>1827</v>
+      </c>
       <c r="G124" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H124" s="6"/>
-      <c r="I124" s="6"/>
-      <c r="J124" s="4"/>
+      <c r="H124" s="6">
+        <v>1</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="J124" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K124" s="8">
         <v>42248</v>
       </c>
@@ -6660,13 +6875,21 @@
       <c r="E125" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F125" s="6"/>
+      <c r="F125" s="6">
+        <v>1827</v>
+      </c>
       <c r="G125" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H125" s="6"/>
-      <c r="I125" s="6"/>
-      <c r="J125" s="4"/>
+      <c r="H125" s="6">
+        <v>1</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="J125" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K125" s="8">
         <v>42248</v>
       </c>
@@ -6682,13 +6905,21 @@
       <c r="E126" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F126" s="6"/>
+      <c r="F126" s="6">
+        <v>1827</v>
+      </c>
       <c r="G126" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H126" s="6"/>
-      <c r="I126" s="6"/>
-      <c r="J126" s="4"/>
+      <c r="H126" s="6">
+        <v>1</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="J126" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K126" s="8">
         <v>42248</v>
       </c>
@@ -6704,13 +6935,21 @@
       <c r="E127" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F127" s="6"/>
+      <c r="F127" s="6">
+        <v>1814</v>
+      </c>
       <c r="G127" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H127" s="6"/>
-      <c r="I127" s="6"/>
-      <c r="J127" s="4"/>
+      <c r="H127" s="6">
+        <v>2</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="J127" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K127" s="8">
         <v>42248</v>
       </c>
@@ -6726,13 +6965,21 @@
       <c r="E128" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F128" s="6"/>
+      <c r="F128" s="6">
+        <v>1814</v>
+      </c>
       <c r="G128" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H128" s="6"/>
-      <c r="I128" s="6"/>
-      <c r="J128" s="4"/>
+      <c r="H128" s="6">
+        <v>2</v>
+      </c>
+      <c r="I128" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="J128" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K128" s="8">
         <v>42248</v>
       </c>
@@ -6748,13 +6995,21 @@
       <c r="E129" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F129" s="6"/>
+      <c r="F129" s="6">
+        <v>1726</v>
+      </c>
       <c r="G129" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H129" s="6"/>
-      <c r="I129" s="6"/>
-      <c r="J129" s="4"/>
+      <c r="H129" s="6">
+        <v>5</v>
+      </c>
+      <c r="I129" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="J129" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K129" s="8">
         <v>42248</v>
       </c>
@@ -6770,13 +7025,21 @@
       <c r="E130" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F130" s="6"/>
+      <c r="F130" s="6">
+        <v>1726</v>
+      </c>
       <c r="G130" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H130" s="6"/>
-      <c r="I130" s="6"/>
-      <c r="J130" s="4"/>
+      <c r="H130" s="6">
+        <v>5</v>
+      </c>
+      <c r="I130" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="J130" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K130" s="8">
         <v>42248</v>
       </c>
@@ -6792,13 +7055,21 @@
       <c r="E131" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F131" s="6"/>
+      <c r="F131" s="6">
+        <v>1726</v>
+      </c>
       <c r="G131" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H131" s="6"/>
-      <c r="I131" s="6"/>
-      <c r="J131" s="4"/>
+      <c r="H131" s="6">
+        <v>5</v>
+      </c>
+      <c r="I131" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="J131" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K131" s="8">
         <v>42248</v>
       </c>
@@ -6814,13 +7085,21 @@
       <c r="E132" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F132" s="6"/>
+      <c r="F132" s="6">
+        <v>1319</v>
+      </c>
       <c r="G132" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H132" s="6"/>
-      <c r="I132" s="6"/>
-      <c r="J132" s="4"/>
+      <c r="H132" s="6">
+        <v>3</v>
+      </c>
+      <c r="I132" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="J132" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K132" s="8">
         <v>42248</v>
       </c>
@@ -6836,13 +7115,21 @@
       <c r="E133" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F133" s="6"/>
+      <c r="F133" s="6">
+        <v>1319</v>
+      </c>
       <c r="G133" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H133" s="6"/>
-      <c r="I133" s="6"/>
-      <c r="J133" s="4"/>
+      <c r="H133" s="6">
+        <v>3</v>
+      </c>
+      <c r="I133" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="J133" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K133" s="8">
         <v>42248</v>
       </c>
@@ -6858,13 +7145,21 @@
       <c r="E134" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F134" s="6"/>
+      <c r="F134" s="6">
+        <v>1819</v>
+      </c>
       <c r="G134" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H134" s="6"/>
-      <c r="I134" s="6"/>
-      <c r="J134" s="4"/>
+      <c r="H134" s="6">
+        <v>3</v>
+      </c>
+      <c r="I134" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="J134" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K134" s="8">
         <v>42248</v>
       </c>
@@ -6880,13 +7175,21 @@
       <c r="E135" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F135" s="6"/>
+      <c r="F135" s="6">
+        <v>1819</v>
+      </c>
       <c r="G135" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H135" s="6"/>
-      <c r="I135" s="6"/>
-      <c r="J135" s="4"/>
+      <c r="H135" s="6">
+        <v>3</v>
+      </c>
+      <c r="I135" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="J135" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K135" s="8">
         <v>42248</v>
       </c>
@@ -6902,13 +7205,21 @@
       <c r="E136" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F136" s="6"/>
-      <c r="G136" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H136" s="6"/>
-      <c r="I136" s="6"/>
-      <c r="J136" s="4"/>
+      <c r="F136" s="16">
+        <v>1819</v>
+      </c>
+      <c r="G136" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H136" s="18">
+        <v>3</v>
+      </c>
+      <c r="I136" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="J136" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K136" s="8">
         <v>42248</v>
       </c>
@@ -9414,20 +9725,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N291"/>
+  <dimension ref="A3:N303"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A287" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="F296" sqref="F296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14">
@@ -9493,7 +9808,9 @@
       <c r="G5" s="1">
         <v>8821</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="14">
@@ -9527,7 +9844,9 @@
       <c r="G6" s="1">
         <v>8822</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="14">
@@ -17049,12 +17368,18 @@
       <c r="A250" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B250" s="1"/>
+      <c r="B250" s="1">
+        <v>1804</v>
+      </c>
       <c r="C250" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D250" s="1"/>
-      <c r="E250" s="1"/>
+      <c r="D250" s="1">
+        <v>2</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>403</v>
+      </c>
       <c r="F250" s="1" t="s">
         <v>99</v>
       </c>
@@ -17127,12 +17452,18 @@
       <c r="A253" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B253" s="1"/>
+      <c r="B253" s="1">
+        <v>1791</v>
+      </c>
       <c r="C253" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D253" s="1"/>
-      <c r="E253" s="1"/>
+      <c r="D253" s="1">
+        <v>3</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>404</v>
+      </c>
       <c r="F253" s="1" t="s">
         <v>99</v>
       </c>
@@ -17205,12 +17536,18 @@
       <c r="A256" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B256" s="1"/>
+      <c r="B256" s="1">
+        <v>1820</v>
+      </c>
       <c r="C256" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D256" s="1"/>
-      <c r="E256" s="1"/>
+      <c r="D256" s="1">
+        <v>2</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="F256" s="1" t="s">
         <v>99</v>
       </c>
@@ -17283,12 +17620,18 @@
       <c r="A259" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B259" s="1"/>
+      <c r="B259" s="1">
+        <v>1733</v>
+      </c>
       <c r="C259" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D259" s="1"/>
-      <c r="E259" s="1"/>
+      <c r="D259" s="1">
+        <v>3</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="F259" s="1" t="s">
         <v>99</v>
       </c>
@@ -17361,12 +17704,18 @@
       <c r="A262" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B262" s="1"/>
+      <c r="B262" s="1">
+        <v>1813</v>
+      </c>
       <c r="C262" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D262" s="1"/>
-      <c r="E262" s="1"/>
+      <c r="D262" s="1">
+        <v>2</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="F262" s="1" t="s">
         <v>99</v>
       </c>
@@ -17439,12 +17788,18 @@
       <c r="A265" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B265" s="1"/>
+      <c r="B265" s="1">
+        <v>1790</v>
+      </c>
       <c r="C265" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D265" s="1"/>
-      <c r="E265" s="1"/>
+      <c r="D265" s="1">
+        <v>2</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>408</v>
+      </c>
       <c r="F265" s="1" t="s">
         <v>99</v>
       </c>
@@ -17465,12 +17820,18 @@
       <c r="A266" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B266" s="1"/>
+      <c r="B266" s="1">
+        <v>1790</v>
+      </c>
       <c r="C266" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D266" s="1"/>
-      <c r="E266" s="1"/>
+      <c r="D266" s="1">
+        <v>2</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>408</v>
+      </c>
       <c r="F266" s="1" t="s">
         <v>100</v>
       </c>
@@ -17517,12 +17878,18 @@
       <c r="A268" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B268" s="1"/>
+      <c r="B268" s="1">
+        <v>1346</v>
+      </c>
       <c r="C268" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D268" s="1"/>
-      <c r="E268" s="1"/>
+      <c r="D268" s="1">
+        <v>4</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>409</v>
+      </c>
       <c r="F268" s="1" t="s">
         <v>99</v>
       </c>
@@ -17543,12 +17910,18 @@
       <c r="A269" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B269" s="1"/>
+      <c r="B269" s="1">
+        <v>1346</v>
+      </c>
       <c r="C269" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D269" s="1"/>
-      <c r="E269" s="1"/>
+      <c r="D269" s="1">
+        <v>4</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>409</v>
+      </c>
       <c r="F269" s="1" t="s">
         <v>100</v>
       </c>
@@ -17595,12 +17968,18 @@
       <c r="A271" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B271" s="1"/>
+      <c r="B271" s="1">
+        <v>1526</v>
+      </c>
       <c r="C271" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D271" s="1"/>
-      <c r="E271" s="1"/>
+      <c r="D271" s="1">
+        <v>2</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>410</v>
+      </c>
       <c r="F271" s="1" t="s">
         <v>99</v>
       </c>
@@ -17673,12 +18052,18 @@
       <c r="A274" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B274" s="1"/>
+      <c r="B274" s="1">
+        <v>1118</v>
+      </c>
       <c r="C274" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D274" s="1"/>
-      <c r="E274" s="1"/>
+      <c r="D274" s="1">
+        <v>2</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>411</v>
+      </c>
       <c r="F274" s="1" t="s">
         <v>99</v>
       </c>
@@ -17751,12 +18136,18 @@
       <c r="A277" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B277" s="1"/>
+      <c r="B277" s="1">
+        <v>1147</v>
+      </c>
       <c r="C277" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D277" s="1"/>
-      <c r="E277" s="1"/>
+      <c r="D277" s="1">
+        <v>3</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="F277" s="1" t="s">
         <v>99</v>
       </c>
@@ -17829,12 +18220,18 @@
       <c r="A280" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B280" s="1"/>
+      <c r="B280" s="1">
+        <v>1509</v>
+      </c>
       <c r="C280" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D280" s="1"/>
-      <c r="E280" s="1"/>
+      <c r="D280" s="1">
+        <v>5</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>413</v>
+      </c>
       <c r="F280" s="1" t="s">
         <v>99</v>
       </c>
@@ -17907,12 +18304,18 @@
       <c r="A283" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B283" s="1"/>
+      <c r="B283" s="1">
+        <v>1702</v>
+      </c>
       <c r="C283" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D283" s="1"/>
-      <c r="E283" s="1"/>
+      <c r="D283" s="1">
+        <v>4</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="F283" s="1" t="s">
         <v>99</v>
       </c>
@@ -17985,12 +18388,18 @@
       <c r="A286" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B286" s="1"/>
+      <c r="B286" s="1">
+        <v>1716</v>
+      </c>
       <c r="C286" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D286" s="1"/>
-      <c r="E286" s="1"/>
+      <c r="D286" s="1">
+        <v>5</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="F286" s="1" t="s">
         <v>99</v>
       </c>
@@ -18063,12 +18472,18 @@
       <c r="A289" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B289" s="1"/>
+      <c r="B289" s="1">
+        <v>1685</v>
+      </c>
       <c r="C289" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D289" s="1"/>
-      <c r="E289" s="1"/>
+      <c r="D289" s="1">
+        <v>4</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>416</v>
+      </c>
       <c r="F289" s="1" t="s">
         <v>99</v>
       </c>
@@ -18136,6 +18551,300 @@
       <c r="L291" s="1"/>
       <c r="M291" s="1"/>
       <c r="N291" s="1"/>
+    </row>
+    <row r="292" spans="1:14">
+      <c r="A292" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B292" s="1">
+        <v>1350</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D292" s="1">
+        <v>3</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G292" s="1">
+        <v>9108</v>
+      </c>
+      <c r="H292" s="1"/>
+      <c r="I292" s="1"/>
+      <c r="J292" s="1"/>
+      <c r="K292" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14">
+      <c r="A293" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B293" s="1"/>
+      <c r="C293" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D293" s="1"/>
+      <c r="E293" s="1"/>
+      <c r="F293" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G293" s="1">
+        <v>9109</v>
+      </c>
+      <c r="H293" s="1"/>
+      <c r="I293" s="1"/>
+      <c r="J293" s="1"/>
+      <c r="K293" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14">
+      <c r="A294" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B294" s="1"/>
+      <c r="C294" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D294" s="1"/>
+      <c r="E294" s="1"/>
+      <c r="F294" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G294" s="1">
+        <v>9110</v>
+      </c>
+      <c r="H294" s="1"/>
+      <c r="I294" s="1"/>
+      <c r="J294" s="1"/>
+      <c r="K294" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14">
+      <c r="A295" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B295" s="1">
+        <v>1507</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D295" s="1">
+        <v>3</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G295" s="1">
+        <v>9111</v>
+      </c>
+      <c r="H295" s="1"/>
+      <c r="I295" s="1"/>
+      <c r="J295" s="1"/>
+      <c r="K295" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14">
+      <c r="A296" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B296" s="1"/>
+      <c r="C296" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D296" s="1"/>
+      <c r="E296" s="1"/>
+      <c r="F296" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G296" s="1">
+        <v>9112</v>
+      </c>
+      <c r="H296" s="1"/>
+      <c r="I296" s="1"/>
+      <c r="J296" s="1"/>
+      <c r="K296" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14">
+      <c r="A297" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B297" s="1"/>
+      <c r="C297" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D297" s="1"/>
+      <c r="E297" s="1"/>
+      <c r="F297" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G297" s="1">
+        <v>9113</v>
+      </c>
+      <c r="H297" s="1"/>
+      <c r="I297" s="1"/>
+      <c r="J297" s="1"/>
+      <c r="K297" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14">
+      <c r="A298" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B298" s="1">
+        <v>1789</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D298" s="1">
+        <v>2</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G298" s="1">
+        <v>9114</v>
+      </c>
+      <c r="H298" s="1"/>
+      <c r="I298" s="1"/>
+      <c r="J298" s="1"/>
+      <c r="K298" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14">
+      <c r="A299" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B299" s="1"/>
+      <c r="C299" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D299" s="1"/>
+      <c r="E299" s="1"/>
+      <c r="F299" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G299" s="1">
+        <v>9115</v>
+      </c>
+      <c r="H299" s="1"/>
+      <c r="I299" s="1"/>
+      <c r="J299" s="1"/>
+      <c r="K299" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14">
+      <c r="A300" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B300" s="1"/>
+      <c r="C300" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D300" s="1"/>
+      <c r="E300" s="1"/>
+      <c r="F300" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G300" s="1">
+        <v>9116</v>
+      </c>
+      <c r="H300" s="1"/>
+      <c r="I300" s="1"/>
+      <c r="J300" s="1"/>
+      <c r="K300" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14">
+      <c r="A301" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B301" s="1"/>
+      <c r="C301" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D301" s="1"/>
+      <c r="E301" s="1"/>
+      <c r="F301" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G301" s="1">
+        <v>9117</v>
+      </c>
+      <c r="H301" s="1"/>
+      <c r="I301" s="1"/>
+      <c r="J301" s="1"/>
+      <c r="K301" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14">
+      <c r="A302" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B302" s="1"/>
+      <c r="C302" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D302" s="1"/>
+      <c r="E302" s="1"/>
+      <c r="F302" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G302" s="1">
+        <v>9118</v>
+      </c>
+      <c r="H302" s="1"/>
+      <c r="I302" s="1"/>
+      <c r="J302" s="1"/>
+      <c r="K302" s="14">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14">
+      <c r="A303" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B303" s="1"/>
+      <c r="C303" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D303" s="1"/>
+      <c r="E303" s="1"/>
+      <c r="F303" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G303" s="1">
+        <v>9119</v>
+      </c>
+      <c r="H303" s="1"/>
+      <c r="I303" s="1"/>
+      <c r="J303" s="1"/>
+      <c r="K303" s="14">
+        <v>42248</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
CR 11 change history done - WG nb created
</commit_message>
<xml_diff>
--- a/etc/ap242/AP242ed2_CR11_WG_Numbers.xlsx
+++ b/etc/ap242/AP242ed2_CR11_WG_Numbers.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="429">
   <si>
     <t>N8573</t>
   </si>
@@ -1326,6 +1326,21 @@
   </si>
   <si>
     <t>tessellated_geometry</t>
+  </si>
+  <si>
+    <t>composite_constituent_shape</t>
+  </si>
+  <si>
+    <t>composite_surface</t>
+  </si>
+  <si>
+    <t>constructive_solid_geometry_2d</t>
+  </si>
+  <si>
+    <t>construction_geometry</t>
+  </si>
+  <si>
+    <t>contextual_shape_positioning</t>
   </si>
 </sst>
 </file>
@@ -1453,8 +1468,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="591">
+  <cellStyleXfs count="613">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2075,7 +2112,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="591">
+  <cellStyles count="613">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2371,6 +2408,17 @@
     <cellStyle name="Lien hypertexte" xfId="585" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="587" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="611" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2666,6 +2714,17 @@
     <cellStyle name="Lien hypertexte visité" xfId="586" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="588" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="612" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2997,8 +3056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E106" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+    <sheetView tabSelected="1" topLeftCell="E43" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0"/>
@@ -5807,13 +5866,21 @@
       <c r="E87" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F87" s="6"/>
+      <c r="F87" s="6">
+        <v>1767</v>
+      </c>
       <c r="G87" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="4"/>
+      <c r="H87" s="6">
+        <v>4</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K87" s="8">
         <v>42248</v>
       </c>
@@ -5829,13 +5896,21 @@
       <c r="E88" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F88" s="6"/>
+      <c r="F88" s="6">
+        <v>1767</v>
+      </c>
       <c r="G88" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H88" s="6"/>
-      <c r="I88" s="6"/>
-      <c r="J88" s="4"/>
+      <c r="H88" s="6">
+        <v>4</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K88" s="8">
         <v>42248</v>
       </c>
@@ -5851,13 +5926,21 @@
       <c r="E89" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F89" s="6"/>
+      <c r="F89" s="6">
+        <v>1525</v>
+      </c>
       <c r="G89" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H89" s="6"/>
-      <c r="I89" s="6"/>
-      <c r="J89" s="4"/>
+      <c r="H89" s="6">
+        <v>2</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K89" s="8">
         <v>42248</v>
       </c>
@@ -5873,13 +5956,21 @@
       <c r="E90" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F90" s="6"/>
+      <c r="F90" s="6">
+        <v>1131</v>
+      </c>
       <c r="G90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H90" s="6"/>
-      <c r="I90" s="6"/>
-      <c r="J90" s="4"/>
+      <c r="H90" s="6">
+        <v>5</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K90" s="8">
         <v>42248</v>
       </c>
@@ -5895,13 +5986,21 @@
       <c r="E91" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F91" s="6"/>
+      <c r="F91" s="6">
+        <v>1131</v>
+      </c>
       <c r="G91" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="4"/>
+      <c r="H91" s="6">
+        <v>5</v>
+      </c>
+      <c r="I91" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="K91" s="8">
         <v>42248</v>
       </c>
@@ -5917,13 +6016,21 @@
       <c r="E92" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F92" s="6"/>
+      <c r="F92" s="6">
+        <v>1731</v>
+      </c>
       <c r="G92" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="4"/>
+      <c r="H92" s="6">
+        <v>4</v>
+      </c>
+      <c r="I92" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K92" s="8">
         <v>42248</v>
       </c>
@@ -5939,13 +6046,21 @@
       <c r="E93" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F93" s="6"/>
+      <c r="F93" s="6">
+        <v>1027</v>
+      </c>
       <c r="G93" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H93" s="6"/>
-      <c r="I93" s="6"/>
-      <c r="J93" s="4"/>
+      <c r="H93" s="6">
+        <v>7</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K93" s="8">
         <v>42248</v>
       </c>
@@ -5961,13 +6076,21 @@
       <c r="E94" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F94" s="6"/>
+      <c r="F94" s="6">
+        <v>1027</v>
+      </c>
       <c r="G94" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="4"/>
+      <c r="H94" s="6">
+        <v>7</v>
+      </c>
+      <c r="I94" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="K94" s="8">
         <v>42248</v>
       </c>
@@ -5983,13 +6106,21 @@
       <c r="E95" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F95" s="6"/>
+      <c r="F95" s="6">
+        <v>1660</v>
+      </c>
       <c r="G95" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="4"/>
+      <c r="H95" s="6">
+        <v>4</v>
+      </c>
+      <c r="I95" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="K95" s="8">
         <v>42248</v>
       </c>
@@ -6018,7 +6149,7 @@
         <v>325</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K96" s="8">
         <v>42248</v>
@@ -6048,7 +6179,7 @@
         <v>325</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K97" s="8">
         <v>42248</v>
@@ -6066,19 +6197,19 @@
         <v>97</v>
       </c>
       <c r="F98" s="6">
-        <v>1660</v>
+        <v>1809</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H98" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K98" s="8">
         <v>42248</v>
@@ -6108,7 +6239,7 @@
         <v>326</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K99" s="8">
         <v>42248</v>
@@ -6126,19 +6257,19 @@
         <v>97</v>
       </c>
       <c r="F100" s="6">
-        <v>1809</v>
+        <v>1130</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H100" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K100" s="8">
         <v>42248</v>
@@ -6168,7 +6299,7 @@
         <v>327</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K101" s="8">
         <v>42248</v>
@@ -6186,19 +6317,19 @@
         <v>97</v>
       </c>
       <c r="F102" s="6">
-        <v>1130</v>
+        <v>1232</v>
       </c>
       <c r="G102" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H102" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K102" s="8">
         <v>42248</v>
@@ -6228,7 +6359,7 @@
         <v>328</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K103" s="8">
         <v>42248</v>
@@ -6246,19 +6377,19 @@
         <v>97</v>
       </c>
       <c r="F104" s="6">
-        <v>1232</v>
+        <v>1628</v>
       </c>
       <c r="G104" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H104" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K104" s="8">
         <v>42248</v>
@@ -6288,7 +6419,7 @@
         <v>329</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K105" s="8">
         <v>42248</v>
@@ -6318,7 +6449,7 @@
         <v>329</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K106" s="8">
         <v>42248</v>
@@ -6336,7 +6467,7 @@
         <v>97</v>
       </c>
       <c r="F107" s="6">
-        <v>1628</v>
+        <v>1050</v>
       </c>
       <c r="G107" s="5" t="s">
         <v>98</v>
@@ -6345,10 +6476,10 @@
         <v>6</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="J107" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K107" s="8">
         <v>42248</v>
@@ -6366,16 +6497,16 @@
         <v>97</v>
       </c>
       <c r="F108" s="6">
-        <v>1050</v>
+        <v>1744</v>
       </c>
       <c r="G108" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H108" s="6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I108" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="J108" s="4" t="s">
         <v>99</v>
@@ -6396,7 +6527,7 @@
         <v>97</v>
       </c>
       <c r="F109" s="6">
-        <v>1744</v>
+        <v>1122</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>98</v>
@@ -6405,7 +6536,7 @@
         <v>4</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="J109" s="4" t="s">
         <v>99</v>
@@ -6438,7 +6569,7 @@
         <v>332</v>
       </c>
       <c r="J110" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K110" s="8">
         <v>42248</v>
@@ -6456,7 +6587,7 @@
         <v>97</v>
       </c>
       <c r="F111" s="6">
-        <v>1122</v>
+        <v>1312</v>
       </c>
       <c r="G111" s="5" t="s">
         <v>98</v>
@@ -6465,10 +6596,10 @@
         <v>4</v>
       </c>
       <c r="I111" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="J111" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K111" s="8">
         <v>42248</v>
@@ -6498,7 +6629,7 @@
         <v>333</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K112" s="8">
         <v>42248</v>
@@ -6516,7 +6647,7 @@
         <v>97</v>
       </c>
       <c r="F113" s="6">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="G113" s="5" t="s">
         <v>98</v>
@@ -6525,10 +6656,10 @@
         <v>4</v>
       </c>
       <c r="I113" s="6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J113" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K113" s="8">
         <v>42248</v>
@@ -6558,7 +6689,7 @@
         <v>334</v>
       </c>
       <c r="J114" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K114" s="8">
         <v>42248</v>
@@ -6576,19 +6707,19 @@
         <v>97</v>
       </c>
       <c r="F115" s="6">
-        <v>1309</v>
+        <v>1005</v>
       </c>
       <c r="G115" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H115" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I115" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J115" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K115" s="8">
         <v>42248</v>
@@ -6618,7 +6749,7 @@
         <v>335</v>
       </c>
       <c r="J116" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K116" s="8">
         <v>42248</v>
@@ -6636,19 +6767,19 @@
         <v>97</v>
       </c>
       <c r="F117" s="6">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H117" s="6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I117" s="6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K117" s="8">
         <v>42248</v>
@@ -6678,7 +6809,7 @@
         <v>336</v>
       </c>
       <c r="J118" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K118" s="8">
         <v>42248</v>
@@ -6708,7 +6839,7 @@
         <v>336</v>
       </c>
       <c r="J119" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K119" s="8">
         <v>42248</v>
@@ -6726,19 +6857,19 @@
         <v>97</v>
       </c>
       <c r="F120" s="6">
-        <v>1004</v>
+        <v>1527</v>
       </c>
       <c r="G120" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H120" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I120" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="J120" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K120" s="8">
         <v>42248</v>
@@ -6756,7 +6887,7 @@
         <v>97</v>
       </c>
       <c r="F121" s="6">
-        <v>1527</v>
+        <v>1064</v>
       </c>
       <c r="G121" s="5" t="s">
         <v>98</v>
@@ -6765,7 +6896,7 @@
         <v>2</v>
       </c>
       <c r="I121" s="6" t="s">
-        <v>337</v>
+        <v>398</v>
       </c>
       <c r="J121" s="4" t="s">
         <v>99</v>
@@ -6786,7 +6917,7 @@
         <v>97</v>
       </c>
       <c r="F122" s="6">
-        <v>1064</v>
+        <v>1788</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>98</v>
@@ -6795,7 +6926,7 @@
         <v>2</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J122" s="4" t="s">
         <v>99</v>
@@ -6816,16 +6947,16 @@
         <v>97</v>
       </c>
       <c r="F123" s="6">
-        <v>1788</v>
+        <v>1827</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H123" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J123" s="4" t="s">
         <v>99</v>
@@ -6858,7 +6989,7 @@
         <v>400</v>
       </c>
       <c r="J124" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K124" s="8">
         <v>42248</v>
@@ -6888,7 +7019,7 @@
         <v>400</v>
       </c>
       <c r="J125" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K125" s="8">
         <v>42248</v>
@@ -6906,19 +7037,19 @@
         <v>97</v>
       </c>
       <c r="F126" s="6">
-        <v>1827</v>
+        <v>1814</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H126" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I126" s="6" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="J126" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K126" s="8">
         <v>42248</v>
@@ -6948,7 +7079,7 @@
         <v>401</v>
       </c>
       <c r="J127" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K127" s="8">
         <v>42248</v>
@@ -6966,19 +7097,19 @@
         <v>97</v>
       </c>
       <c r="F128" s="6">
-        <v>1814</v>
+        <v>1726</v>
       </c>
       <c r="G128" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H128" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I128" s="6" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J128" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K128" s="8">
         <v>42248</v>
@@ -7008,7 +7139,7 @@
         <v>402</v>
       </c>
       <c r="J129" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K129" s="8">
         <v>42248</v>
@@ -7038,7 +7169,7 @@
         <v>402</v>
       </c>
       <c r="J130" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K130" s="8">
         <v>42248</v>
@@ -7056,19 +7187,19 @@
         <v>97</v>
       </c>
       <c r="F131" s="6">
-        <v>1726</v>
+        <v>1319</v>
       </c>
       <c r="G131" s="5" t="s">
         <v>98</v>
       </c>
       <c r="H131" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I131" s="6" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="J131" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K131" s="8">
         <v>42248</v>
@@ -7098,7 +7229,7 @@
         <v>422</v>
       </c>
       <c r="J132" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K132" s="8">
         <v>42248</v>
@@ -7116,7 +7247,7 @@
         <v>97</v>
       </c>
       <c r="F133" s="6">
-        <v>1319</v>
+        <v>1819</v>
       </c>
       <c r="G133" s="5" t="s">
         <v>98</v>
@@ -7125,10 +7256,10 @@
         <v>3</v>
       </c>
       <c r="I133" s="6" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="J133" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K133" s="8">
         <v>42248</v>
@@ -7158,7 +7289,7 @@
         <v>423</v>
       </c>
       <c r="J134" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K134" s="8">
         <v>42248</v>
@@ -7175,20 +7306,20 @@
       <c r="E135" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F135" s="6">
+      <c r="F135" s="16">
         <v>1819</v>
       </c>
-      <c r="G135" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H135" s="6">
+      <c r="G135" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H135" s="18">
         <v>3</v>
       </c>
-      <c r="I135" s="6" t="s">
+      <c r="I135" s="18" t="s">
         <v>423</v>
       </c>
       <c r="J135" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K135" s="8">
         <v>42248</v>
@@ -7204,21 +7335,6 @@
       <c r="D136" s="7"/>
       <c r="E136" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="F136" s="16">
-        <v>1819</v>
-      </c>
-      <c r="G136" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="H136" s="18">
-        <v>3</v>
-      </c>
-      <c r="I136" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="J136" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="K136" s="8">
         <v>42248</v>
@@ -9727,7 +9843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N303"/>
   <sheetViews>
-    <sheetView topLeftCell="A287" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="F296" sqref="F296"/>
     </sheetView>
   </sheetViews>

</xml_diff>